<commit_message>
Beta fixes to warning handling system
</commit_message>
<xml_diff>
--- a/input_data/2011/cli.bigrocks_&_milestones/v2.milestone.journeys.a6i.xlsx
+++ b/input_data/2011/cli.bigrocks_&_milestones/v2.milestone.journeys.a6i.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\test_db\input_data\2011\cli.bigrocks_&amp;_milestones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D12997-6F74-481E-859A-DEB0011C1738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF898A55-85EA-420C-8BAE-824B51A9A100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Posting Label" sheetId="1" r:id="rId1"/>
@@ -122,9 +122,6 @@
     <t>modernization-milestone</t>
   </si>
   <si>
-    <t>H2:L30</t>
-  </si>
-  <si>
     <t>Posting Label</t>
   </si>
   <si>
@@ -288,6 +285,9 @@
   </si>
   <si>
     <t>modernization-milestone.1</t>
+  </si>
+  <si>
+    <t>H2:K30</t>
   </si>
 </sst>
 </file>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -744,7 +744,7 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
@@ -894,7 +894,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
@@ -915,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -935,123 +935,123 @@
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.45">
       <c r="H1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.45">
       <c r="H2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.45">
       <c r="H3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.45">
       <c r="H4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.45">
       <c r="H5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.45">
       <c r="H6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="2:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="H7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -1061,18 +1061,18 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -1081,35 +1081,35 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -1119,18 +1119,18 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -1139,15 +1139,15 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -1159,17 +1159,17 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K16" s="4"/>
     </row>
@@ -1179,13 +1179,13 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -1193,17 +1193,17 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B18" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -1213,40 +1213,40 @@
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>